<commit_message>
tidying gitignore, reverting 4_analyse to ne for ni
</commit_message>
<xml_diff>
--- a/doc/wind_database_metadata.xlsx
+++ b/doc/wind_database_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spann\Documents\Research\reynolds_scales_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spann\Documents\Research\Code repos\reynolds_scales_project\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC8BDD0-5937-483E-BC11-7C72C6332686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90222990-BEFC-4CE4-A824-4048AA1592F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{60C75D1D-90E2-4A5F-AB16-E1D6DF71A971}"/>
+    <workbookView xWindow="-23385" yWindow="45" windowWidth="15375" windowHeight="8325" xr2:uid="{60C75D1D-90E2-4A5F-AB16-E1D6DF71A971}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="141">
   <si>
     <t>Variables for Wind database</t>
   </si>
@@ -197,9 +197,6 @@
     <t>Uncertainty of Taylor timescale (corrected)</t>
   </si>
   <si>
-    <t>Taylor timescale (Kevin's method)</t>
-  </si>
-  <si>
     <t>Standard deviation of linear fit x correction factor</t>
   </si>
   <si>
@@ -221,9 +218,6 @@
     <t>Chuychai method with correction based on qk</t>
   </si>
   <si>
-    <t>ttk</t>
-  </si>
-  <si>
     <t>Power-law fit to power spectrum over range 0.01 &lt; f &lt; 0.2</t>
   </si>
   <si>
@@ -284,9 +278,6 @@
     <t>Wind (wi_h2_mfi): BGSE_2</t>
   </si>
   <si>
-    <t>Raw variable</t>
-  </si>
-  <si>
     <t>Correlation timescale, 1/e method</t>
   </si>
   <si>
@@ -305,12 +296,6 @@
     <t>Integral of ACF up to x-value where ACF falls to 0</t>
   </si>
   <si>
-    <t>Naïve estimate: fit to single range of up to 20 lags</t>
-  </si>
-  <si>
-    <t>For checking against Kevin's earlier results</t>
-  </si>
-  <si>
     <t>5.31*(ne**-1/2)</t>
   </si>
   <si>
@@ -374,9 +359,6 @@
     <t>Values outside the range 0-1000 are set to missing</t>
   </si>
   <si>
-    <t>Analytical variable</t>
-  </si>
-  <si>
     <t>Numerical variable</t>
   </si>
   <si>
@@ -386,18 +368,9 @@
     <t>Calculated from high-res Wind data, with mean calculated from entire dataset. Typically then divide by B0 (sqrt of sum of squared mean components) to get variable of interest</t>
   </si>
   <si>
-    <t>1 wk average</t>
-  </si>
-  <si>
     <t>Debye length (electron)</t>
   </si>
   <si>
-    <t>Wang2017 used 0.005-0.2Hz</t>
-  </si>
-  <si>
-    <t>Wang2017 used 0.5-1.4Hz</t>
-  </si>
-  <si>
     <t xml:space="preserve">From NRL formulary (converting nT to Gauss). </t>
   </si>
   <si>
@@ -407,9 +380,6 @@
     <t>(7.43e-3)*(Te**1/2)(ne**-1/2)</t>
   </si>
   <si>
-    <t>"+ energy (acov at 0 lag), c.f. Mark's values"</t>
-  </si>
-  <si>
     <t>(2.38e-5)*(Te**1/2)*((Bwind*e-5)**-1)</t>
   </si>
   <si>
@@ -450,6 +420,45 @@
   </si>
   <si>
     <t>Should be around 0.4-0.5Hz (Weygand2007), corresponding to distances of 600-1000km</t>
+  </si>
+  <si>
+    <t>11.1 (4520km)</t>
+  </si>
+  <si>
+    <t>7.1 (3000km)</t>
+  </si>
+  <si>
+    <t>2303 (900000km)</t>
+  </si>
+  <si>
+    <t>2193 (900000km)</t>
+  </si>
+  <si>
+    <t>2117 (900000km)</t>
+  </si>
+  <si>
+    <t>From NRL formulary (converting cm to km and nT to Gauss). Correlation with magnetic field should be about 1/r</t>
+  </si>
+  <si>
+    <t>Wang2017 used 0.005-0.2Hz. Theory tells us should be -5/3 (1.67)</t>
+  </si>
+  <si>
+    <t>Wang2017 used 0.5-1.4Hz. Shown to be about -8/3 (-2.67)</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>re_tb</t>
+  </si>
+  <si>
+    <t>Reynolds number (spectral break method)</t>
+  </si>
+  <si>
+    <t>Primary variable</t>
+  </si>
+  <si>
+    <t>Derived variable</t>
   </si>
 </sst>
 </file>
@@ -541,7 +550,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -623,17 +632,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -687,7 +685,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -703,9 +701,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
@@ -715,12 +712,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="3" applyFill="1" applyBorder="1"/>
@@ -738,11 +735,11 @@
     <xf numFmtId="1" fontId="2" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="6" borderId="6" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1006,7 +1003,7 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{69A8CBD7-495C-4F77-9807-78FEB8E3AF0F}" name="Name in database" dataDxfId="5" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{D6A57239-58B9-4C96-93D7-C08DD9CBA495}" name="Full name" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{E29AF60E-8C37-476C-9021-82D4040D9DF6}" name="1 wk average" dataDxfId="3" dataCellStyle="40% - Accent3"/>
+    <tableColumn id="4" xr3:uid="{E29AF60E-8C37-476C-9021-82D4040D9DF6}" name="Average" dataDxfId="3" dataCellStyle="40% - Accent3"/>
     <tableColumn id="3" xr3:uid="{A5AF20BE-333B-48B4-AC25-68960254473D}" name="Unit" dataDxfId="2" dataCellStyle="40% - Accent3"/>
     <tableColumn id="6" xr3:uid="{6FEA0C9A-F1C6-4A66-9476-C4AE4F69ED82}" name="Dataset OR derivation method" dataDxfId="1" dataCellStyle="40% - Accent3"/>
     <tableColumn id="8" xr3:uid="{7BBB7C73-A571-43CF-A5A8-5DD1CD903E7D}" name="Notes" dataDxfId="0"/>
@@ -1312,20 +1309,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{993E126D-618E-4F8A-9C35-3E793C167672}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="F21" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="8" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.42578125" customWidth="1"/>
     <col min="6" max="6" width="255.7109375" bestFit="1" customWidth="1"/>
@@ -1333,52 +1330,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
+      <c r="A2" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
-        <v>82</v>
+      <c r="A4" s="34" t="s">
+        <v>139</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
-        <v>112</v>
+      <c r="A5" s="35" t="s">
+        <v>140</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
-        <v>113</v>
+      <c r="A6" s="36" t="s">
+        <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1389,459 +1386,459 @@
         <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="19" t="s">
+      <c r="C11" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E11" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="19" t="s">
+      <c r="F11" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>93</v>
+      <c r="A12" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>88</v>
       </c>
       <c r="C12" s="6">
-        <v>6.8</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F12" s="28"/>
+        <v>89</v>
+      </c>
+      <c r="F12" s="27"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="C13" s="33">
-        <v>6.5</v>
-      </c>
-      <c r="D13" s="32" t="s">
+      <c r="A13" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="32">
+        <v>5.7</v>
+      </c>
+      <c r="D13" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="F13" s="33" t="s">
-        <v>110</v>
+      <c r="E13" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="21" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="6">
-        <v>2.2000000000000002</v>
+        <v>2.1</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="6">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="27">
+        <v>4.8</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="25"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="27">
+        <v>13.9</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="28">
-        <v>3.9</v>
-      </c>
-      <c r="D16" s="26" t="s">
+      <c r="F17" s="25"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="27">
+        <v>5.5</v>
+      </c>
+      <c r="D18" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="F16" s="26"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="28">
-        <v>13.5</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" s="26"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="28">
-        <v>4.8</v>
-      </c>
-      <c r="D18" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>99</v>
+      <c r="E18" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="28">
-        <v>17.3</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="F19" s="26"/>
+      <c r="C19" s="27">
+        <v>15.4</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="25"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="38">
-        <v>1.39</v>
+      <c r="C20" s="37">
+        <v>1.6</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="39">
-        <v>68</v>
+      <c r="C21" s="38">
+        <v>66.3</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="22" t="s">
         <v>31</v>
       </c>
       <c r="C22" s="11">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>43</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="22" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="9">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="40">
-        <v>0.52</v>
+      <c r="C24" s="39">
+        <v>0.93</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="40">
-        <v>0.85</v>
+      <c r="C25" s="39">
+        <v>0.92</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="39">
-        <v>74</v>
+      <c r="C26" s="38">
+        <v>111.8</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>117</v>
+        <v>95</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>110</v>
       </c>
       <c r="C27" s="9">
-        <v>1.6E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="22" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="11">
-        <v>6.3</v>
+        <v>5.8</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>45</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>56</v>
       </c>
       <c r="C29" s="14">
-        <v>-1.65</v>
+        <v>-1.68</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>40</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>57</v>
       </c>
       <c r="C30" s="14">
-        <v>-2.86</v>
+        <v>-2.63</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>40</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="23" t="s">
         <v>38</v>
       </c>
       <c r="C31" s="14">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>27</v>
@@ -1850,44 +1847,44 @@
         <v>44</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C32" s="14">
-        <v>1710</v>
+      <c r="B32" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>130</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>27</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33" s="14">
-        <v>1664</v>
+      <c r="B33" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>131</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F33" s="14"/>
     </row>
@@ -1895,17 +1892,17 @@
       <c r="A34" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34" s="14">
-        <v>1739</v>
+      <c r="B34" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>132</v>
       </c>
       <c r="D34" s="13" t="s">
         <v>27</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F34" s="14"/>
     </row>
@@ -1913,17 +1910,17 @@
       <c r="A35" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="14">
-        <v>9.8000000000000007</v>
+      <c r="C35" s="14" t="s">
+        <v>128</v>
       </c>
       <c r="D35" s="13" t="s">
         <v>27</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F35" s="14"/>
     </row>
@@ -1931,11 +1928,11 @@
       <c r="A36" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="23" t="s">
         <v>50</v>
       </c>
       <c r="C36" s="14">
-        <v>0.08</v>
+        <v>0.13</v>
       </c>
       <c r="D36" s="13" t="s">
         <v>27</v>
@@ -1949,17 +1946,17 @@
       <c r="A37" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="14">
-        <v>7.5</v>
+      <c r="C37" s="14" t="s">
+        <v>129</v>
       </c>
       <c r="D37" s="13" t="s">
         <v>27</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F37" s="14"/>
     </row>
@@ -1967,78 +1964,74 @@
       <c r="A38" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C38" s="14">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D38" s="13" t="s">
         <v>27</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F38" s="14"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B39" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" s="17">
-        <v>19</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>90</v>
+      <c r="A39" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39" s="44"/>
+      <c r="D39" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="46" t="s">
-        <v>129</v>
-      </c>
-      <c r="B40" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="C40" s="45"/>
-      <c r="D40" s="16" t="s">
+      <c r="A40" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" s="44">
+        <v>4520000</v>
+      </c>
+      <c r="D40" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E40" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>135</v>
-      </c>
+      <c r="E40" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="F40" s="41"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="B41" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="C41" s="45"/>
-      <c r="D41" s="16" t="s">
+      <c r="A41" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="B41" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="C41" s="44">
+        <v>194000</v>
+      </c>
+      <c r="D41" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E41" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="F41" s="42"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="41" t="s">
-        <v>123</v>
-      </c>
+      <c r="E41" s="15"/>
+      <c r="F41" s="41"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
tidying code, extending metadata
</commit_message>
<xml_diff>
--- a/doc/wind_database_metadata.xlsx
+++ b/doc/wind_database_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spann\Documents\Research\Code repos\reynolds_scales_project\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90222990-BEFC-4CE4-A824-4048AA1592F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26F0219-9D66-465C-AC0C-78F32F6053E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23385" yWindow="45" windowWidth="15375" windowHeight="8325" xr2:uid="{60C75D1D-90E2-4A5F-AB16-E1D6DF71A971}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{60C75D1D-90E2-4A5F-AB16-E1D6DF71A971}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,9 +419,6 @@
     <t>Corr scale in km should be around 1-3,000,000km</t>
   </si>
   <si>
-    <t>Should be around 0.4-0.5Hz (Weygand2007), corresponding to distances of 600-1000km</t>
-  </si>
-  <si>
     <t>11.1 (4520km)</t>
   </si>
   <si>
@@ -459,6 +456,9 @@
   </si>
   <si>
     <t>Derived variable</t>
+  </si>
+  <si>
+    <t>Should be around 0.4-0.5Hz (Weygand2007), corresponding to distances of 600-1000km. Roberts2022 says 10s</t>
   </si>
 </sst>
 </file>
@@ -1312,10 +1312,10 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="F23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,7 +1356,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
         <v>103</v>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B5" t="s">
         <v>101</v>
@@ -1386,7 +1386,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>21</v>
@@ -1627,7 +1627,7 @@
         <v>114</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1807,7 +1807,7 @@
         <v>60</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1827,7 +1827,7 @@
         <v>61</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1847,7 +1847,7 @@
         <v>44</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1858,7 +1858,7 @@
         <v>80</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>27</v>
@@ -1878,7 +1878,7 @@
         <v>82</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>27</v>
@@ -1896,7 +1896,7 @@
         <v>81</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D34" s="13" t="s">
         <v>27</v>
@@ -1914,7 +1914,7 @@
         <v>49</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D35" s="13" t="s">
         <v>27</v>
@@ -1950,7 +1950,7 @@
         <v>51</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D37" s="13" t="s">
         <v>27</v>
@@ -2016,10 +2016,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="B41" s="43" t="s">
         <v>137</v>
-      </c>
-      <c r="B41" s="43" t="s">
-        <v>138</v>
       </c>
       <c r="C41" s="44">
         <v>194000</v>

</xml_diff>